<commit_message>
Expand bltu, bgeu, sltu, sltiu
</commit_message>
<xml_diff>
--- a/lab6/General_Lab/code_table.xlsx
+++ b/lab6/General_Lab/code_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18213\Sources\COD_Lab\lab6\General_Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2842BA83-24E3-4883-AA0A-7F9308FDE29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C915608B-E385-47C6-A91D-04CDBC334AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13230" yWindow="3560" windowWidth="28800" windowHeight="15410" activeTab="1" xr2:uid="{FEA91FBE-1A34-46E3-9397-A1B48428F097}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{FEA91FBE-1A34-46E3-9397-A1B48428F097}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="107">
   <si>
     <t>指令名称</t>
   </si>
@@ -346,31 +346,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>求和</t>
-    </r>
-  </si>
-  <si>
-    <t>平均值</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>汇总</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>计数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>MemRead</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -436,6 +411,34 @@
   </si>
   <si>
     <t>BranchSel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>bgeu</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1110011</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>bltu</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>sltiu</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>sltu</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unsigned</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -928,7 +931,7 @@
         <v>80</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>81</v>
@@ -1076,7 +1079,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -1572,7 +1575,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>22</v>
@@ -1861,10 +1864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A749061C-363F-489E-86DD-842DA141FE7F}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1874,7 +1877,7 @@
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1903,10 +1906,13 @@
         <v>73</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1937,10 +1943,13 @@
       <c r="J2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>34</v>
@@ -1955,10 +1964,10 @@
         <v>66</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>69</v>
@@ -1969,8 +1978,11 @@
       <c r="J3" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1987,7 +1999,7 @@
         <v>29</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>31</v>
@@ -2001,10 +2013,13 @@
       <c r="J4" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -2016,27 +2031,30 @@
         <v>64</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -2045,19 +2063,19 @@
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
@@ -2065,10 +2083,13 @@
       <c r="J6" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>34</v>
@@ -2077,16 +2098,16 @@
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>69</v>
@@ -2097,10 +2118,13 @@
       <c r="J7" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
@@ -2109,19 +2133,19 @@
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="I8" s="4">
         <v>0</v>
@@ -2129,10 +2153,13 @@
       <c r="J8" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>34</v>
@@ -2144,13 +2171,13 @@
         <v>64</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>32</v>
@@ -2161,42 +2188,48 @@
       <c r="J9" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1100011</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>35</v>
@@ -2205,10 +2238,10 @@
         <v>1100011</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>11</v>
@@ -2223,12 +2256,15 @@
         <v>0</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>35</v>
@@ -2237,10 +2273,10 @@
         <v>1100011</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>100</v>
+        <v>64</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>11</v>
@@ -2255,12 +2291,15 @@
         <v>0</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>35</v>
@@ -2269,10 +2308,10 @@
         <v>1100011</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>65</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>100</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>11</v>
@@ -2281,39 +2320,77 @@
         <v>31</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1100011</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2">
-        <v>10</v>
+        <v>102</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="I16" s="4">
         <v>0</v>
@@ -2321,77 +2398,51 @@
       <c r="J16" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="I17" s="4">
         <v>0</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>6</v>
+      </c>
+      <c r="B19" s="2">
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>22</v>
@@ -2400,48 +2451,51 @@
         <v>71</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>88</v>
+        <v>27</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="I19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>10</v>
+      </c>
+      <c r="B20" s="2">
+        <v>10</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
@@ -2449,10 +2503,13 @@
       <c r="J20" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>36</v>
@@ -2464,13 +2521,13 @@
         <v>71</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>90</v>
+        <v>66</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>64</v>
@@ -2481,10 +2538,13 @@
       <c r="J21" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>36</v>
@@ -2493,30 +2553,33 @@
         <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>64</v>
       </c>
       <c r="I22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>36</v>
@@ -2528,27 +2591,30 @@
         <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>64</v>
       </c>
       <c r="I23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>36</v>
@@ -2560,13 +2626,13 @@
         <v>71</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>64</v>
@@ -2577,150 +2643,165 @@
       <c r="J24" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" s="4">
-        <v>0</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="4">
-        <v>0</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1101111</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="4">
-        <v>0</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="2">
-        <v>1100111</v>
+      <c r="C30" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>7</v>
@@ -2729,17 +2810,160 @@
         <v>30</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I30" s="4">
-        <v>0</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I45" s="1"/>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1101111</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1100111</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>